<commit_message>
Dataset: add category, dataset and apply to facility and scorecard
</commit_message>
<xml_diff>
--- a/lib/samples/assets/csv/primary_schools.xlsx
+++ b/lib/samples/assets/csv/primary_schools.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/www/csc-web/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/www/csc-web/lib/samples/assets/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Koh Kong" sheetId="1" r:id="rId1"/>
@@ -97,8 +97,8 @@
           <t>if school code present, then we will find for this code to update or create new record following this school code.
 In case school code is not present, then the system will used the generate a new school code for this record following the format.
 commune_code_auto-increment_id_from_previous_commune_code
-e.g: commune code is 100101 -&gt; and this school is the first in this commune -&gt;
-school code is 100101_1
+e.g: commune code is 090101 -&gt; and this school is the first in this commune -&gt;
+school code is 090101_1
 	-Sokly Heng</t>
         </r>
       </text>
@@ -110,18 +110,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
-    <t>commune_code</t>
-  </si>
-  <si>
-    <t>school_code</t>
-  </si>
-  <si>
-    <t>school_name_en</t>
-  </si>
-  <si>
-    <t>school_name_km</t>
-  </si>
-  <si>
     <t>090101</t>
   </si>
   <si>
@@ -180,6 +168,18 @@
   </si>
   <si>
     <t>ឆ្លូង</t>
+  </si>
+  <si>
+    <t>location_id</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>name_en</t>
+  </si>
+  <si>
+    <t>name_km</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -519,16 +519,16 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -552,45 +552,45 @@
     </row>
     <row r="2" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -607,7 +607,7 @@
   <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -620,16 +620,16 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -653,44 +653,44 @@
     </row>
     <row r="2" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>18</v>
-      </c>
       <c r="C3" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>